<commit_message>
updated WBS, Pert Matrix, Plan documents
</commit_message>
<xml_diff>
--- a/TERM3/T3B1-ICTPMG613-Manage_ICT_project_plan/2-ICTPMG613-Assessment_Task 2/PERT-chart.xlsx
+++ b/TERM3/T3B1-ICTPMG613-Manage_ICT_project_plan/2-ICTPMG613-Assessment_Task 2/PERT-chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manue\Documents\Assessments\TERM3\T3B1-ICTPMG613-Manage_ICT_project_plan\2-ICTPMG613-Assessment_Task 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC2FDDA-A7CF-46AC-AF0F-4A45255AD8C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A26CB3-91C3-4D84-9928-445F0D31F710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2E7573F3-6188-4FA9-9041-50436B486355}"/>
   </bookViews>
@@ -290,9 +290,6 @@
     <t>68,62</t>
   </si>
   <si>
-    <t>Lack of clarity in requirements</t>
-  </si>
-  <si>
     <t>Delays in internal review</t>
   </si>
   <si>
@@ -510,6 +507,9 @@
   </si>
   <si>
     <t>Dev</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Understanding requirements, and lack of software fuctionalities </t>
   </si>
 </sst>
 </file>
@@ -1057,7 +1057,7 @@
   <dimension ref="A1:H70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1077,19 +1077,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="11" t="s">
         <v>156</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>157</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>1</v>
@@ -1123,7 +1123,7 @@
         <v>3</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>84</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1151,7 +1151,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1179,7 +1179,7 @@
         <v>2</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1207,7 +1207,7 @@
         <v>3</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1235,7 +1235,7 @@
         <v>4</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1263,7 +1263,7 @@
         <v>5</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1291,7 +1291,7 @@
         <v>6</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1319,7 +1319,7 @@
         <v>7</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1347,7 +1347,7 @@
         <v>8</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1375,7 +1375,7 @@
         <v>9</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1403,7 +1403,7 @@
         <v>10</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -1431,7 +1431,7 @@
         <v>10</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1459,7 +1459,7 @@
         <v>17</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1487,7 +1487,7 @@
         <v>13</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1515,7 +1515,7 @@
         <v>11</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1543,7 +1543,7 @@
         <v>15</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1571,7 +1571,7 @@
         <v>16</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1599,7 +1599,7 @@
         <v>17</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1627,7 +1627,7 @@
         <v>13</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1655,7 +1655,7 @@
         <v>19</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1683,7 +1683,7 @@
         <v>20</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1711,7 +1711,7 @@
         <v>27</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -1739,7 +1739,7 @@
         <v>22</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1767,7 +1767,7 @@
         <v>23</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -1795,7 +1795,7 @@
         <v>23</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1823,7 +1823,7 @@
         <v>32</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1851,7 +1851,7 @@
         <v>8</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1879,7 +1879,7 @@
         <v>27</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1907,7 +1907,7 @@
         <v>28</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1935,7 +1935,7 @@
         <v>8</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1963,7 +1963,7 @@
         <v>30</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1991,7 +1991,7 @@
         <v>31</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -2019,7 +2019,7 @@
         <v>29</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -2047,7 +2047,7 @@
         <v>33</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -2075,7 +2075,7 @@
         <v>42</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2103,7 +2103,7 @@
         <v>35</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -2131,7 +2131,7 @@
         <v>36</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -2159,7 +2159,7 @@
         <v>46</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2187,7 +2187,7 @@
         <v>38</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -2215,7 +2215,7 @@
         <v>49</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2243,7 +2243,7 @@
         <v>40</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2271,7 +2271,7 @@
         <v>41</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -2299,7 +2299,7 @@
         <v>42</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -2327,7 +2327,7 @@
         <v>43</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -2355,7 +2355,7 @@
         <v>43</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -2383,7 +2383,7 @@
         <v>43</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
@@ -2411,7 +2411,7 @@
         <v>57</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2439,7 +2439,7 @@
         <v>59</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2467,7 +2467,7 @@
         <v>59</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2495,7 +2495,7 @@
         <v>62</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -2523,7 +2523,7 @@
         <v>50</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2551,7 +2551,7 @@
         <v>51</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -2579,7 +2579,7 @@
         <v>52</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -2607,7 +2607,7 @@
         <v>53</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2635,7 +2635,7 @@
         <v>54</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2663,7 +2663,7 @@
         <v>55</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2691,7 +2691,7 @@
         <v>56</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2719,7 +2719,7 @@
         <v>57</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -2747,7 +2747,7 @@
         <v>58</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -2775,7 +2775,7 @@
         <v>57</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2803,7 +2803,7 @@
         <v>60</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -2831,7 +2831,7 @@
         <v>61</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -2859,7 +2859,7 @@
         <v>76</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -2887,7 +2887,7 @@
         <v>63</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2915,7 +2915,7 @@
         <v>64</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -2943,7 +2943,7 @@
         <v>65</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2971,7 +2971,7 @@
         <v>66</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2999,7 +2999,7 @@
         <v>67</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -3027,7 +3027,7 @@
         <v>83</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>